<commit_message>
M3 Cord Production System #405 - M3.Cord.Production.App re-implements #205.
</commit_message>
<xml_diff>
--- a/Documents/Cord/Cord Documents/4001 condition S-1.xlsx
+++ b/Documents/Cord/Cord Documents/4001 condition S-1.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toraygroup01-my.sharepoint.com/personal/paiboon_mongkollert_e5_mail_toray/Documents/Budget Traeback Cord 2022/DCC/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E24C196-CC59-43D8-94B6-6CE5889A4A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C8181F49-4471-4B7A-AC51-AF8739DF39AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="KT9S71 (Production)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -490,11 +484,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="187" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1354,9 +1348,6 @@
   </cellStyleXfs>
   <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1388,64 +1379,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1455,50 +1400,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1524,32 +1431,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -1573,19 +1456,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1599,17 +1470,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1617,122 +1479,20 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1757,46 +1517,75 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1808,46 +1597,251 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{13D855BB-4314-43B0-A3B8-DCF073921020}"/>
-    <cellStyle name="ปกติ_Original" xfId="1" xr:uid="{E7518226-C8B2-4927-8DBC-9A577BB20255}"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ_Original" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1882,7 +1876,7 @@
         <xdr:cNvPr id="2" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83453A2D-96AE-45C6-B4BA-555A77021B18}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83453A2D-96AE-45C6-B4BA-555A77021B18}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1929,7 +1923,7 @@
         <xdr:cNvPr id="3" name="Line 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8607D0A4-1157-4506-B5A1-C39B78759738}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8607D0A4-1157-4506-B5A1-C39B78759738}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1976,7 +1970,7 @@
         <xdr:cNvPr id="4" name="Line 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5AC21C7-A837-4509-9C17-5DD454324DF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5AC21C7-A837-4509-9C17-5DD454324DF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2023,7 +2017,7 @@
         <xdr:cNvPr id="5" name="Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098A5C90-760C-4C57-BCB1-ABFE1DBBB0A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{098A5C90-760C-4C57-BCB1-ABFE1DBBB0A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2072,7 +2066,7 @@
         <xdr:cNvPr id="6" name="Rectangle 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC375A52-7A04-4F83-A567-D1A68DEF8520}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CC375A52-7A04-4F83-A567-D1A68DEF8520}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2121,7 +2115,7 @@
         <xdr:cNvPr id="7" name="Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C5E1F05-8536-453E-A0FB-40C155A30B93}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4C5E1F05-8536-453E-A0FB-40C155A30B93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2170,7 +2164,7 @@
         <xdr:cNvPr id="8" name="Rectangle 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C5E92C6-5F94-46A1-837C-DEA08CC9ED7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2C5E92C6-5F94-46A1-837C-DEA08CC9ED7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2247,7 +2241,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2299,7 +2293,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2493,831 +2487,816 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE90393-9EC0-46FF-9C3C-0706F8F31C96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="21.5" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="2"/>
-    <col min="11" max="11" width="10.1796875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9.81640625" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="5.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.21875" style="1"/>
+    <col min="11" max="11" width="10.21875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.77734375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A1" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="188"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" s="13" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A2" s="6" t="s">
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" s="12" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8">
         <v>44955</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:11" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="G3" s="14"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="16" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" ht="3.75" customHeight="1" thickBot="1">
+      <c r="G3" s="13"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" ht="28.5" customHeight="1" thickTop="1">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="189" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21" t="s">
+      <c r="F4" s="190"/>
+      <c r="G4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="191" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A5" s="24" t="s">
+      <c r="I4" s="192"/>
+    </row>
+    <row r="5" spans="1:11" ht="28.5" customHeight="1">
+      <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="172" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="173"/>
+      <c r="E5" s="193" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30" t="s">
+      <c r="F5" s="194"/>
+      <c r="G5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="195" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="K5" s="2" t="s">
+      <c r="I5" s="196"/>
+      <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:11" ht="39.75" customHeight="1">
+      <c r="A6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="172" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="33" t="s">
+      <c r="D6" s="173"/>
+      <c r="E6" s="174" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35" t="s">
+      <c r="F6" s="175"/>
+      <c r="G6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="176" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="37"/>
-    </row>
-    <row r="7" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A7" s="38" t="s">
+      <c r="I6" s="177"/>
+    </row>
+    <row r="7" spans="1:11" ht="28.5" customHeight="1" thickBot="1">
+      <c r="A7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42"/>
-    </row>
-    <row r="8" spans="1:11" s="44" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="178"/>
+      <c r="I7" s="179"/>
+    </row>
+    <row r="8" spans="1:11" s="27" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="180" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="47"/>
-    </row>
-    <row r="9" spans="1:11" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A9" s="48" t="s">
+      <c r="I8" s="181"/>
+    </row>
+    <row r="9" spans="1:11" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="182" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51" t="s">
+      <c r="B9" s="183"/>
+      <c r="C9" s="183"/>
+      <c r="D9" s="184"/>
+      <c r="E9" s="185" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="54"/>
-    </row>
-    <row r="10" spans="1:11" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="55" t="s">
+      <c r="G9" s="187"/>
+      <c r="H9" s="187"/>
+      <c r="I9" s="103"/>
+    </row>
+    <row r="10" spans="1:11" ht="20.25" customHeight="1" thickTop="1">
+      <c r="A10" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="144" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60" t="s">
+      <c r="C10" s="145"/>
+      <c r="D10" s="146"/>
+      <c r="E10" s="186"/>
+      <c r="F10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="61"/>
-      <c r="H10" s="62" t="s">
+      <c r="G10" s="31"/>
+      <c r="H10" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="63"/>
-    </row>
-    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A11" s="64">
+      <c r="I10" s="148"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A11" s="131">
         <v>1</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="67" t="s">
+      <c r="E11" s="33"/>
+      <c r="F11" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="68"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="70"/>
-    </row>
-    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A12" s="64"/>
-      <c r="B12" s="65" t="s">
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A12" s="131"/>
+      <c r="B12" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="66"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A13" s="64"/>
-      <c r="B13" s="24" t="s">
+      <c r="E12" s="33"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A13" s="131"/>
+      <c r="B13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="75" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="76"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="78"/>
-    </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A14" s="79">
+      <c r="G13" s="43"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A14" s="118">
         <v>2</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="80" t="s">
+      <c r="E14" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="71" t="s">
+      <c r="F14" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="68"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="70"/>
-    </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A15" s="81"/>
-      <c r="B15" s="24" t="s">
+      <c r="G14" s="35"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A15" s="149"/>
+      <c r="B15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="83" t="s">
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="78"/>
-    </row>
-    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A16" s="64">
+      <c r="G15" s="43"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+    </row>
+    <row r="16" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A16" s="131">
         <v>3</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="71" t="s">
+      <c r="E16" s="33"/>
+      <c r="F16" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="68"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="70"/>
-    </row>
-    <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="64"/>
-      <c r="B17" s="24" t="s">
+      <c r="G16" s="35"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="37"/>
+    </row>
+    <row r="17" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A17" s="131"/>
+      <c r="B17" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="75" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="76"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="78"/>
-    </row>
-    <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A18" s="64">
+      <c r="G17" s="43"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+    </row>
+    <row r="18" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A18" s="131">
         <v>4</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="84">
+      <c r="E18" s="33"/>
+      <c r="F18" s="168">
         <v>217</v>
       </c>
-      <c r="G18" s="85"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="70"/>
-    </row>
-    <row r="19" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A19" s="64"/>
-      <c r="B19" s="24" t="s">
+      <c r="G18" s="169"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="37"/>
+    </row>
+    <row r="19" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A19" s="131"/>
+      <c r="B19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="78"/>
-    </row>
-    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A20" s="64">
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="170"/>
+      <c r="G19" s="171"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+    </row>
+    <row r="20" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A20" s="131">
         <v>5</v>
       </c>
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="70"/>
-    </row>
-    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A21" s="64"/>
-      <c r="B21" s="24" t="s">
+      <c r="E20" s="33"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="37"/>
+    </row>
+    <row r="21" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A21" s="131"/>
+      <c r="B21" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="90" t="s">
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="91"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="78"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A22" s="64">
+      <c r="G21" s="50"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+    </row>
+    <row r="22" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A22" s="131">
         <v>6</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="70"/>
-    </row>
-    <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A23" s="64"/>
-      <c r="B23" s="24" t="s">
+      <c r="E22" s="33"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="37"/>
+    </row>
+    <row r="23" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A23" s="131"/>
+      <c r="B23" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="92" t="s">
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="93"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="78"/>
-    </row>
-    <row r="24" spans="1:13" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A24" s="79">
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="45"/>
+    </row>
+    <row r="24" spans="1:13" s="55" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A24" s="118">
         <v>7</v>
       </c>
-      <c r="B24" s="95" t="s">
+      <c r="B24" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="97"/>
-      <c r="F24" s="98" t="s">
+      <c r="E24" s="56"/>
+      <c r="F24" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="99"/>
-      <c r="H24" s="100"/>
-      <c r="I24" s="70"/>
-    </row>
-    <row r="25" spans="1:13" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A25" s="81"/>
-      <c r="B25" s="95" t="s">
+      <c r="G24" s="160"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="37"/>
+    </row>
+    <row r="25" spans="1:13" s="55" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A25" s="149"/>
+      <c r="B25" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="97"/>
-      <c r="F25" s="101" t="s">
+      <c r="E25" s="56"/>
+      <c r="F25" s="161" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="102"/>
-      <c r="H25" s="103" t="s">
+      <c r="G25" s="162"/>
+      <c r="H25" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="I25" s="104" t="s">
+      <c r="I25" s="59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A26" s="79">
+    <row r="26" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A26" s="118">
         <v>8</v>
       </c>
-      <c r="B26" s="105" t="s">
+      <c r="B26" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="106"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="108"/>
-      <c r="F26" s="109" t="s">
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="110"/>
-      <c r="H26" s="111"/>
-      <c r="I26" s="112"/>
-    </row>
-    <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A27" s="113"/>
-      <c r="B27" s="114" t="s">
+      <c r="G26" s="165"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="65"/>
+    </row>
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A27" s="163"/>
+      <c r="B27" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="115"/>
-      <c r="D27" s="115"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="117" t="s">
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="118"/>
-      <c r="H27" s="119" t="s">
+      <c r="G27" s="167"/>
+      <c r="H27" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="I27" s="120" t="s">
+      <c r="I27" s="70" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="A28" s="121"/>
-      <c r="B28" s="56" t="s">
+    <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1">
+      <c r="A28" s="71"/>
+      <c r="B28" s="144" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="60" t="s">
+      <c r="C28" s="145"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="61"/>
-      <c r="H28" s="62" t="s">
+      <c r="G28" s="31"/>
+      <c r="H28" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="63"/>
-    </row>
-    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A29" s="122">
+      <c r="I28" s="148"/>
+    </row>
+    <row r="29" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A29" s="119">
         <v>9</v>
       </c>
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="80" t="s">
+      <c r="E29" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="123" t="s">
+      <c r="F29" s="197" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="124"/>
-      <c r="H29" s="125" t="s">
+      <c r="G29" s="152"/>
+      <c r="H29" s="155" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="126"/>
-    </row>
-    <row r="30" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A30" s="81"/>
-      <c r="B30" s="24" t="s">
+      <c r="I29" s="156"/>
+    </row>
+    <row r="30" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A30" s="149"/>
+      <c r="B30" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="127"/>
-      <c r="G30" s="128"/>
-      <c r="H30" s="129"/>
-      <c r="I30" s="130"/>
-      <c r="K30" s="2">
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="151"/>
+      <c r="F30" s="153"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="157"/>
+      <c r="I30" s="158"/>
+      <c r="K30" s="1">
         <v>120</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="1">
         <v>105</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="1">
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A31" s="64">
+    <row r="31" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A31" s="131">
         <v>10</v>
       </c>
-      <c r="B31" s="65" t="s">
+      <c r="B31" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="66"/>
-      <c r="F31" s="131" t="s">
+      <c r="E31" s="33"/>
+      <c r="F31" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="G31" s="132"/>
-      <c r="H31" s="133" t="s">
+      <c r="G31" s="133"/>
+      <c r="H31" s="136" t="s">
         <v>65</v>
       </c>
-      <c r="I31" s="134"/>
-      <c r="K31" s="2">
+      <c r="I31" s="137"/>
+      <c r="K31" s="1">
         <v>3800</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="1">
         <v>3830</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="1">
         <v>3770</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A32" s="64"/>
-      <c r="B32" s="24" t="s">
+    <row r="32" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A32" s="131"/>
+      <c r="B32" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="135"/>
-      <c r="G32" s="136"/>
-      <c r="H32" s="137"/>
-      <c r="I32" s="138"/>
-    </row>
-    <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A33" s="64">
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="134"/>
+      <c r="G32" s="135"/>
+      <c r="H32" s="138"/>
+      <c r="I32" s="139"/>
+    </row>
+    <row r="33" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A33" s="131">
         <v>11</v>
       </c>
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="66"/>
-      <c r="F33" s="139" t="s">
+      <c r="E33" s="33"/>
+      <c r="F33" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="140"/>
-      <c r="H33" s="133" t="s">
+      <c r="G33" s="141"/>
+      <c r="H33" s="136" t="s">
         <v>72</v>
       </c>
-      <c r="I33" s="134"/>
-      <c r="K33" s="2">
+      <c r="I33" s="137"/>
+      <c r="K33" s="1">
         <f>K31/K30</f>
         <v>31.666666666666668</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="1">
         <f t="shared" ref="L33:M33" si="0">L31/L30</f>
         <v>36.476190476190474</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="1">
         <f t="shared" si="0"/>
         <v>27.925925925925927</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A34" s="64"/>
-      <c r="B34" s="24" t="s">
+    <row r="34" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A34" s="131"/>
+      <c r="B34" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="141"/>
-      <c r="G34" s="142"/>
-      <c r="H34" s="137"/>
-      <c r="I34" s="138"/>
-    </row>
-    <row r="35" spans="1:13" s="96" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A35" s="79">
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="143"/>
+      <c r="H34" s="138"/>
+      <c r="I34" s="139"/>
+    </row>
+    <row r="35" spans="1:13" s="55" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A35" s="118">
         <v>12</v>
       </c>
-      <c r="B35" s="105" t="s">
+      <c r="B35" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="143"/>
-      <c r="D35" s="143"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="145" t="s">
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="120" t="s">
         <v>75</v>
       </c>
-      <c r="G35" s="146"/>
-      <c r="H35" s="147"/>
-      <c r="I35" s="148"/>
-      <c r="L35" s="96">
+      <c r="G35" s="121"/>
+      <c r="H35" s="122"/>
+      <c r="I35" s="123"/>
+      <c r="L35" s="55">
         <f>K33-M33</f>
         <v>3.7407407407407405</v>
       </c>
-      <c r="M35" s="96">
+      <c r="M35" s="55">
         <f>L33-K33</f>
         <v>4.8095238095238066</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A36" s="122"/>
-      <c r="B36" s="95" t="s">
+    <row r="36" spans="1:13" s="55" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A36" s="119"/>
+      <c r="B36" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="E36" s="97"/>
-      <c r="F36" s="149"/>
-      <c r="G36" s="150"/>
-      <c r="H36" s="151"/>
-      <c r="I36" s="152"/>
-    </row>
-    <row r="37" spans="1:13" s="96" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A37" s="153"/>
-      <c r="B37" s="154"/>
-      <c r="C37" s="155"/>
-      <c r="D37" s="155"/>
-      <c r="E37" s="156"/>
-      <c r="F37" s="157"/>
-      <c r="G37" s="158"/>
-      <c r="H37" s="157"/>
-      <c r="I37" s="159"/>
-    </row>
-    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A38" s="160" t="s">
+      <c r="E36" s="56"/>
+      <c r="F36" s="124"/>
+      <c r="G36" s="125"/>
+      <c r="H36" s="126"/>
+      <c r="I36" s="127"/>
+    </row>
+    <row r="37" spans="1:13" s="55" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="128"/>
+      <c r="G37" s="129"/>
+      <c r="H37" s="128"/>
+      <c r="I37" s="130"/>
+    </row>
+    <row r="38" spans="1:13" ht="21" customHeight="1">
+      <c r="A38" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="161"/>
-      <c r="D38" s="161"/>
-      <c r="E38" s="161"/>
-      <c r="F38" s="162"/>
-      <c r="G38" s="162"/>
-      <c r="H38" s="161"/>
-    </row>
-    <row r="39" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A39" s="163"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="161"/>
-      <c r="D39" s="161"/>
-      <c r="E39" s="161"/>
-      <c r="F39" s="162"/>
-      <c r="G39" s="162"/>
-      <c r="H39" s="161"/>
-    </row>
-    <row r="40" spans="1:13" ht="0.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A40" s="163"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="161"/>
-      <c r="D40" s="161"/>
-      <c r="E40" s="161"/>
-      <c r="F40" s="162"/>
-      <c r="G40" s="162"/>
-      <c r="H40" s="161"/>
-    </row>
-    <row r="41" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A41" s="164" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="79"/>
+    </row>
+    <row r="39" spans="1:13" ht="2.25" customHeight="1">
+      <c r="A39" s="81"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="79"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="80"/>
+      <c r="G39" s="80"/>
+      <c r="H39" s="79"/>
+    </row>
+    <row r="40" spans="1:13" ht="0.75" customHeight="1">
+      <c r="A40" s="81"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="79"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="79"/>
+    </row>
+    <row r="41" spans="1:13" ht="19.5" customHeight="1">
+      <c r="A41" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="165"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="166" t="s">
+      <c r="B41" s="83"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="G41" s="167" t="s">
+      <c r="G41" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="H41" s="168" t="s">
+      <c r="H41" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="I41" s="169"/>
-    </row>
-    <row r="42" spans="1:13" s="175" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A42" s="170" t="s">
+      <c r="I41" s="105"/>
+    </row>
+    <row r="42" spans="1:13" s="90" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A42" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="171"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="172" t="s">
+      <c r="B42" s="87"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="106" t="s">
         <v>83</v>
       </c>
-      <c r="G42" s="173"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="174"/>
-    </row>
-    <row r="43" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A43" s="170" t="s">
+      <c r="G42" s="88"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="89"/>
+    </row>
+    <row r="43" spans="1:13" ht="20.25" customHeight="1">
+      <c r="A43" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="171"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="176"/>
-      <c r="G43" s="177"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="179"/>
-    </row>
-    <row r="44" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A44" s="170" t="s">
+      <c r="B43" s="87"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="107"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="109"/>
+      <c r="I43" s="110"/>
+    </row>
+    <row r="44" spans="1:13" ht="24.75" customHeight="1">
+      <c r="A44" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="171"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="180"/>
-      <c r="G44" s="181" t="s">
+      <c r="B44" s="87"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="108"/>
+      <c r="G44" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="H44" s="182" t="s">
+      <c r="H44" s="111" t="s">
         <v>86</v>
       </c>
-      <c r="I44" s="183"/>
-    </row>
-    <row r="45" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A45" s="170" t="s">
+      <c r="I44" s="112"/>
+    </row>
+    <row r="45" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A45" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="171"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="184" t="s">
+      <c r="B45" s="87"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="G45" s="185"/>
-      <c r="H45" s="186"/>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.75">
-      <c r="A46" s="170" t="s">
+      <c r="G45" s="93"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="14"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="171"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="187"/>
-      <c r="G46" s="185"/>
-      <c r="H46" s="188"/>
-      <c r="I46" s="78"/>
-    </row>
-    <row r="47" spans="1:13" ht="22" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A47" s="189" t="s">
+      <c r="B46" s="87"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="114"/>
+      <c r="G46" s="93"/>
+      <c r="H46" s="95"/>
+      <c r="I46" s="45"/>
+    </row>
+    <row r="47" spans="1:13" ht="21.6" thickBot="1">
+      <c r="A47" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="190"/>
-      <c r="C47" s="191"/>
-      <c r="D47" s="191"/>
-      <c r="E47" s="191"/>
-      <c r="F47" s="192"/>
-      <c r="G47" s="193" t="s">
+      <c r="B47" s="97"/>
+      <c r="C47" s="98"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="98"/>
+      <c r="F47" s="115"/>
+      <c r="G47" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="H47" s="194" t="s">
+      <c r="H47" s="116" t="s">
         <v>92</v>
       </c>
-      <c r="I47" s="195"/>
-    </row>
-    <row r="48" spans="1:13" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="A48" s="196" t="s">
+      <c r="I47" s="117"/>
+    </row>
+    <row r="48" spans="1:13" ht="22.2" thickTop="1" thickBot="1">
+      <c r="A48" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="197"/>
-      <c r="H48" s="52" t="s">
+      <c r="B48" s="101"/>
+      <c r="H48" s="102" t="s">
         <v>94</v>
       </c>
-      <c r="I48" s="54"/>
-    </row>
-    <row r="49" ht="22" thickTop="1" x14ac:dyDescent="0.75"/>
+      <c r="I48" s="103"/>
+    </row>
+    <row r="49" ht="21.6" thickTop="1"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="F31:G32"/>
-    <mergeCell ref="H31:I32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="H33:I34"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:G30"/>
-    <mergeCell ref="H29:I30"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="F27:G27"/>
@@ -3327,22 +3306,37 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="F18:G19"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:G30"/>
+    <mergeCell ref="H29:I30"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="F31:G32"/>
+    <mergeCell ref="H31:I32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="H33:I34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="H47:I47"/>
   </mergeCells>
   <pageMargins left="0.24" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
M3 Cord Production System #451 - M3.Cord.Production.App re-implements #251.
</commit_message>
<xml_diff>
--- a/Documents/Cord/Cord Documents/4001 condition S-1.xlsx
+++ b/Documents/Cord/Cord Documents/4001 condition S-1.xlsx
@@ -1561,238 +1561,39 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1804,37 +1605,236 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1876,7 +1876,7 @@
         <xdr:cNvPr id="2" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83453A2D-96AE-45C6-B4BA-555A77021B18}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83453A2D-96AE-45C6-B4BA-555A77021B18}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1923,7 +1923,7 @@
         <xdr:cNvPr id="3" name="Line 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8607D0A4-1157-4506-B5A1-C39B78759738}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8607D0A4-1157-4506-B5A1-C39B78759738}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1970,7 +1970,7 @@
         <xdr:cNvPr id="4" name="Line 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5AC21C7-A837-4509-9C17-5DD454324DF5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5AC21C7-A837-4509-9C17-5DD454324DF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2017,7 +2017,7 @@
         <xdr:cNvPr id="5" name="Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{098A5C90-760C-4C57-BCB1-ABFE1DBBB0A3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098A5C90-760C-4C57-BCB1-ABFE1DBBB0A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2066,7 +2066,7 @@
         <xdr:cNvPr id="6" name="Rectangle 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CC375A52-7A04-4F83-A567-D1A68DEF8520}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC375A52-7A04-4F83-A567-D1A68DEF8520}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2115,7 +2115,7 @@
         <xdr:cNvPr id="7" name="Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4C5E1F05-8536-453E-A0FB-40C155A30B93}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C5E1F05-8536-453E-A0FB-40C155A30B93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2164,7 +2164,7 @@
         <xdr:cNvPr id="8" name="Rectangle 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2C5E92C6-5F94-46A1-837C-DEA08CC9ED7F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C5E92C6-5F94-46A1-837C-DEA08CC9ED7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2487,7 +2487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2500,8 +2500,8 @@
   </sheetPr>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="21"/>
@@ -2523,10 +2523,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="188"/>
+      <c r="B1" s="102"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
         <v>1</v>
@@ -2566,38 +2566,38 @@
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="189" t="s">
+      <c r="E4" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="190"/>
+      <c r="F4" s="104"/>
       <c r="G4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="191" t="s">
+      <c r="H4" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="192"/>
+      <c r="I4" s="106"/>
     </row>
     <row r="5" spans="1:11" ht="28.5" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="172" t="s">
+      <c r="C5" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="173"/>
-      <c r="E5" s="193" t="s">
+      <c r="D5" s="108"/>
+      <c r="E5" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="194"/>
+      <c r="F5" s="110"/>
       <c r="G5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="195" t="s">
+      <c r="H5" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="196"/>
+      <c r="I5" s="112"/>
       <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2607,21 +2607,21 @@
         <v>15</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="172" t="s">
+      <c r="C6" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174" t="s">
+      <c r="D6" s="108"/>
+      <c r="E6" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="175"/>
+      <c r="F6" s="127"/>
       <c r="G6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="176" t="s">
+      <c r="H6" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="177"/>
+      <c r="I6" s="129"/>
     </row>
     <row r="7" spans="1:11" ht="28.5" customHeight="1" thickBot="1">
       <c r="A7" s="23" t="s">
@@ -2633,8 +2633,8 @@
       <c r="E7" s="25"/>
       <c r="F7" s="13"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="179"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="131"/>
     </row>
     <row r="8" spans="1:11" s="27" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="26" t="s">
@@ -2645,49 +2645,49 @@
       <c r="D8" s="26"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
-      <c r="H8" s="180" t="s">
+      <c r="H8" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="181"/>
+      <c r="I8" s="133"/>
     </row>
     <row r="9" spans="1:11" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="182" t="s">
+      <c r="A9" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="183"/>
-      <c r="C9" s="183"/>
-      <c r="D9" s="184"/>
-      <c r="E9" s="185" t="s">
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="102" t="s">
+      <c r="F9" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="187"/>
-      <c r="H9" s="187"/>
-      <c r="I9" s="103"/>
+      <c r="G9" s="119"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="120"/>
     </row>
     <row r="10" spans="1:11" ht="20.25" customHeight="1" thickTop="1">
       <c r="A10" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="145"/>
-      <c r="D10" s="146"/>
-      <c r="E10" s="186"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="117"/>
       <c r="F10" s="30" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="31"/>
-      <c r="H10" s="147" t="s">
+      <c r="H10" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="148"/>
+      <c r="I10" s="125"/>
     </row>
     <row r="11" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A11" s="131">
+      <c r="A11" s="140">
         <v>1</v>
       </c>
       <c r="B11" s="32" t="s">
@@ -2702,7 +2702,7 @@
       <c r="I11" s="37"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A12" s="131"/>
+      <c r="A12" s="140"/>
       <c r="B12" s="32" t="s">
         <v>32</v>
       </c>
@@ -2713,7 +2713,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A13" s="131"/>
+      <c r="A13" s="140"/>
       <c r="B13" s="19" t="s">
         <v>33</v>
       </c>
@@ -2728,13 +2728,13 @@
       <c r="I13" s="45"/>
     </row>
     <row r="14" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A14" s="118">
+      <c r="A14" s="134">
         <v>2</v>
       </c>
       <c r="B14" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="150" t="s">
+      <c r="E14" s="142" t="s">
         <v>36</v>
       </c>
       <c r="F14" s="38" t="s">
@@ -2745,13 +2745,13 @@
       <c r="I14" s="37"/>
     </row>
     <row r="15" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A15" s="149"/>
+      <c r="A15" s="141"/>
       <c r="B15" s="19" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="151"/>
+      <c r="E15" s="143"/>
       <c r="F15" s="46" t="s">
         <v>39</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="I15" s="45"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A16" s="131">
+      <c r="A16" s="140">
         <v>3</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -2775,7 +2775,7 @@
       <c r="I16" s="37"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A17" s="131"/>
+      <c r="A17" s="140"/>
       <c r="B17" s="19" t="s">
         <v>42</v>
       </c>
@@ -2790,35 +2790,35 @@
       <c r="I17" s="45"/>
     </row>
     <row r="18" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A18" s="131">
+      <c r="A18" s="140">
         <v>4</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="33"/>
-      <c r="F18" s="168">
+      <c r="F18" s="144">
         <v>217</v>
       </c>
-      <c r="G18" s="169"/>
+      <c r="G18" s="145"/>
       <c r="H18" s="39"/>
       <c r="I18" s="37"/>
     </row>
     <row r="19" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A19" s="131"/>
+      <c r="A19" s="140"/>
       <c r="B19" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="41"/>
-      <c r="F19" s="170"/>
-      <c r="G19" s="171"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="147"/>
       <c r="H19" s="44"/>
       <c r="I19" s="45"/>
     </row>
     <row r="20" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A20" s="131">
+      <c r="A20" s="140">
         <v>5</v>
       </c>
       <c r="B20" s="32" t="s">
@@ -2831,7 +2831,7 @@
       <c r="I20" s="37"/>
     </row>
     <row r="21" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A21" s="131"/>
+      <c r="A21" s="140"/>
       <c r="B21" s="19" t="s">
         <v>47</v>
       </c>
@@ -2846,7 +2846,7 @@
       <c r="I21" s="45"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A22" s="131">
+      <c r="A22" s="140">
         <v>6</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -2859,7 +2859,7 @@
       <c r="I22" s="37"/>
     </row>
     <row r="23" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A23" s="131"/>
+      <c r="A23" s="140"/>
       <c r="B23" s="19" t="s">
         <v>50</v>
       </c>
@@ -2874,30 +2874,30 @@
       <c r="I23" s="45"/>
     </row>
     <row r="24" spans="1:13" s="55" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A24" s="118">
+      <c r="A24" s="134">
         <v>7</v>
       </c>
       <c r="B24" s="54" t="s">
         <v>52</v>
       </c>
       <c r="E24" s="56"/>
-      <c r="F24" s="159" t="s">
+      <c r="F24" s="148" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="160"/>
+      <c r="G24" s="149"/>
       <c r="H24" s="57"/>
       <c r="I24" s="37"/>
     </row>
     <row r="25" spans="1:13" s="55" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A25" s="149"/>
+      <c r="A25" s="141"/>
       <c r="B25" s="54" t="s">
         <v>54</v>
       </c>
       <c r="E25" s="56"/>
-      <c r="F25" s="161" t="s">
+      <c r="F25" s="150" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="162"/>
+      <c r="G25" s="151"/>
       <c r="H25" s="58" t="s">
         <v>56</v>
       </c>
@@ -2906,7 +2906,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A26" s="118">
+      <c r="A26" s="134">
         <v>8</v>
       </c>
       <c r="B26" s="60" t="s">
@@ -2915,25 +2915,25 @@
       <c r="C26" s="61"/>
       <c r="D26" s="62"/>
       <c r="E26" s="63"/>
-      <c r="F26" s="164" t="s">
+      <c r="F26" s="136" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="165"/>
+      <c r="G26" s="137"/>
       <c r="H26" s="64"/>
       <c r="I26" s="65"/>
     </row>
     <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A27" s="163"/>
+      <c r="A27" s="135"/>
       <c r="B27" s="66" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="67"/>
       <c r="D27" s="67"/>
       <c r="E27" s="68"/>
-      <c r="F27" s="166" t="s">
+      <c r="F27" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="167"/>
+      <c r="G27" s="139"/>
       <c r="H27" s="69" t="s">
         <v>56</v>
       </c>
@@ -2943,52 +2943,52 @@
     </row>
     <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1">
       <c r="A28" s="71"/>
-      <c r="B28" s="144" t="s">
+      <c r="B28" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="145"/>
-      <c r="D28" s="146"/>
+      <c r="C28" s="122"/>
+      <c r="D28" s="123"/>
       <c r="E28" s="41"/>
       <c r="F28" s="30" t="s">
         <v>28</v>
       </c>
       <c r="G28" s="31"/>
-      <c r="H28" s="147" t="s">
+      <c r="H28" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="148"/>
+      <c r="I28" s="125"/>
     </row>
     <row r="29" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A29" s="119">
+      <c r="A29" s="152">
         <v>9</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="150" t="s">
+      <c r="E29" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="197" t="s">
+      <c r="F29" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="152"/>
-      <c r="H29" s="155" t="s">
+      <c r="G29" s="154"/>
+      <c r="H29" s="157" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="156"/>
+      <c r="I29" s="158"/>
     </row>
     <row r="30" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A30" s="149"/>
+      <c r="A30" s="141"/>
       <c r="B30" s="19" t="s">
         <v>66</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="151"/>
-      <c r="F30" s="153"/>
-      <c r="G30" s="154"/>
-      <c r="H30" s="157"/>
-      <c r="I30" s="158"/>
+      <c r="E30" s="143"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="156"/>
+      <c r="H30" s="159"/>
+      <c r="I30" s="160"/>
       <c r="K30" s="1">
         <v>120</v>
       </c>
@@ -3000,21 +3000,21 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A31" s="131">
+      <c r="A31" s="140">
         <v>10</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>67</v>
       </c>
       <c r="E31" s="33"/>
-      <c r="F31" s="132" t="s">
+      <c r="F31" s="164" t="s">
         <v>68</v>
       </c>
-      <c r="G31" s="133"/>
-      <c r="H31" s="136" t="s">
+      <c r="G31" s="165"/>
+      <c r="H31" s="168" t="s">
         <v>65</v>
       </c>
-      <c r="I31" s="137"/>
+      <c r="I31" s="169"/>
       <c r="K31" s="1">
         <v>3800</v>
       </c>
@@ -3026,34 +3026,34 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A32" s="131"/>
+      <c r="A32" s="140"/>
       <c r="B32" s="19" t="s">
         <v>69</v>
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="40"/>
       <c r="E32" s="41"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="135"/>
-      <c r="H32" s="138"/>
-      <c r="I32" s="139"/>
+      <c r="F32" s="166"/>
+      <c r="G32" s="167"/>
+      <c r="H32" s="170"/>
+      <c r="I32" s="171"/>
     </row>
     <row r="33" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A33" s="131">
+      <c r="A33" s="140">
         <v>11</v>
       </c>
       <c r="B33" s="32" t="s">
         <v>70</v>
       </c>
       <c r="E33" s="33"/>
-      <c r="F33" s="140" t="s">
+      <c r="F33" s="172" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="141"/>
-      <c r="H33" s="136" t="s">
+      <c r="G33" s="173"/>
+      <c r="H33" s="168" t="s">
         <v>72</v>
       </c>
-      <c r="I33" s="137"/>
+      <c r="I33" s="169"/>
       <c r="K33" s="1">
         <f>K31/K30</f>
         <v>31.666666666666668</v>
@@ -3068,20 +3068,20 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A34" s="131"/>
+      <c r="A34" s="140"/>
       <c r="B34" s="19" t="s">
         <v>73</v>
       </c>
       <c r="C34" s="40"/>
       <c r="D34" s="40"/>
       <c r="E34" s="41"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="143"/>
-      <c r="H34" s="138"/>
-      <c r="I34" s="139"/>
+      <c r="F34" s="174"/>
+      <c r="G34" s="175"/>
+      <c r="H34" s="170"/>
+      <c r="I34" s="171"/>
     </row>
     <row r="35" spans="1:13" s="55" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A35" s="118">
+      <c r="A35" s="134">
         <v>12</v>
       </c>
       <c r="B35" s="60" t="s">
@@ -3090,12 +3090,12 @@
       <c r="C35" s="72"/>
       <c r="D35" s="72"/>
       <c r="E35" s="73"/>
-      <c r="F35" s="120" t="s">
+      <c r="F35" s="176" t="s">
         <v>75</v>
       </c>
-      <c r="G35" s="121"/>
-      <c r="H35" s="122"/>
-      <c r="I35" s="123"/>
+      <c r="G35" s="177"/>
+      <c r="H35" s="178"/>
+      <c r="I35" s="179"/>
       <c r="L35" s="55">
         <f>K33-M33</f>
         <v>3.7407407407407405</v>
@@ -3106,15 +3106,15 @@
       </c>
     </row>
     <row r="36" spans="1:13" s="55" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="119"/>
+      <c r="A36" s="152"/>
       <c r="B36" s="54" t="s">
         <v>76</v>
       </c>
       <c r="E36" s="56"/>
-      <c r="F36" s="124"/>
-      <c r="G36" s="125"/>
-      <c r="H36" s="126"/>
-      <c r="I36" s="127"/>
+      <c r="F36" s="180"/>
+      <c r="G36" s="181"/>
+      <c r="H36" s="182"/>
+      <c r="I36" s="183"/>
     </row>
     <row r="37" spans="1:13" s="55" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
       <c r="A37" s="74"/>
@@ -3122,10 +3122,10 @@
       <c r="C37" s="76"/>
       <c r="D37" s="76"/>
       <c r="E37" s="77"/>
-      <c r="F37" s="128"/>
-      <c r="G37" s="129"/>
-      <c r="H37" s="128"/>
-      <c r="I37" s="130"/>
+      <c r="F37" s="161"/>
+      <c r="G37" s="162"/>
+      <c r="H37" s="161"/>
+      <c r="I37" s="163"/>
     </row>
     <row r="38" spans="1:13" ht="21" customHeight="1">
       <c r="A38" s="78" t="s">
@@ -3173,10 +3173,10 @@
       <c r="G41" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="H41" s="104" t="s">
+      <c r="H41" s="184" t="s">
         <v>81</v>
       </c>
-      <c r="I41" s="105"/>
+      <c r="I41" s="185"/>
     </row>
     <row r="42" spans="1:13" s="90" customFormat="1" ht="24.75" customHeight="1">
       <c r="A42" s="86" t="s">
@@ -3186,7 +3186,7 @@
       <c r="C42" s="27"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
-      <c r="F42" s="106" t="s">
+      <c r="F42" s="186" t="s">
         <v>83</v>
       </c>
       <c r="G42" s="88"/>
@@ -3201,10 +3201,10 @@
       <c r="C43" s="27"/>
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
-      <c r="F43" s="107"/>
+      <c r="F43" s="187"/>
       <c r="G43" s="91"/>
-      <c r="H43" s="109"/>
-      <c r="I43" s="110"/>
+      <c r="H43" s="189"/>
+      <c r="I43" s="190"/>
     </row>
     <row r="44" spans="1:13" ht="24.75" customHeight="1">
       <c r="A44" s="86" t="s">
@@ -3214,14 +3214,14 @@
       <c r="C44" s="27"/>
       <c r="D44" s="27"/>
       <c r="E44" s="26"/>
-      <c r="F44" s="108"/>
+      <c r="F44" s="188"/>
       <c r="G44" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="H44" s="111" t="s">
+      <c r="H44" s="191" t="s">
         <v>86</v>
       </c>
-      <c r="I44" s="112"/>
+      <c r="I44" s="192"/>
     </row>
     <row r="45" spans="1:13" ht="23.25" customHeight="1">
       <c r="A45" s="86" t="s">
@@ -3231,7 +3231,7 @@
       <c r="C45" s="27"/>
       <c r="D45" s="27"/>
       <c r="E45" s="26"/>
-      <c r="F45" s="113" t="s">
+      <c r="F45" s="193" t="s">
         <v>88</v>
       </c>
       <c r="G45" s="93"/>
@@ -3246,7 +3246,7 @@
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
       <c r="E46" s="26"/>
-      <c r="F46" s="114"/>
+      <c r="F46" s="194"/>
       <c r="G46" s="93"/>
       <c r="H46" s="95"/>
       <c r="I46" s="45"/>
@@ -3259,44 +3259,54 @@
       <c r="C47" s="98"/>
       <c r="D47" s="98"/>
       <c r="E47" s="98"/>
-      <c r="F47" s="115"/>
+      <c r="F47" s="195"/>
       <c r="G47" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="H47" s="116" t="s">
+      <c r="H47" s="196" t="s">
         <v>92</v>
       </c>
-      <c r="I47" s="117"/>
+      <c r="I47" s="197"/>
     </row>
     <row r="48" spans="1:13" ht="22.2" thickTop="1" thickBot="1">
       <c r="A48" s="100" t="s">
         <v>93</v>
       </c>
       <c r="B48" s="101"/>
-      <c r="H48" s="102" t="s">
+      <c r="H48" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="I48" s="103"/>
+      <c r="I48" s="120"/>
     </row>
     <row r="49" ht="21.6" thickTop="1"/>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="F31:G32"/>
+    <mergeCell ref="H31:I32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="H33:I34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:G30"/>
+    <mergeCell ref="H29:I30"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="F27:G27"/>
@@ -3311,32 +3321,22 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:G30"/>
-    <mergeCell ref="H29:I30"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="F31:G32"/>
-    <mergeCell ref="H31:I32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="H33:I34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.24" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
M3 Cord Production System #465 - M3.Cord.Production.App re-implements #265.
</commit_message>
<xml_diff>
--- a/Documents/Cord/Cord Documents/4001 condition S-1.xlsx
+++ b/Documents/Cord/Cord Documents/4001 condition S-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" tabRatio="421"/>
   </bookViews>
   <sheets>
     <sheet name="KT9S71 (Production)" sheetId="1" r:id="rId1"/>
@@ -105,34 +105,7 @@
     <t>BSCBF</t>
   </si>
   <si>
-    <t>Cord structure (โครงสร้างเชือก)</t>
-  </si>
-  <si>
     <t>KT3S71</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> P 1100</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="18"/>
-        <rFont val="Cordia New"/>
-        <family val="2"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <rFont val="Cordia New"/>
-        <family val="2"/>
-      </rPr>
-      <t>//2</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -480,6 +453,34 @@
   <si>
     <t>Retention : 15 year</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> P 1100</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="18"/>
+        <rFont val="Cordia New"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <rFont val="Cordia New"/>
+        <family val="2"/>
+      </rPr>
+      <t>//2</t>
+    </r>
+  </si>
+  <si>
+    <t>Cord structure (โครงสร้างเชือก)
+จริง ๆ คือ Product Item Code</t>
+  </si>
 </sst>
 </file>
 
@@ -488,7 +489,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -535,19 +536,6 @@
       <b/>
       <vertAlign val="superscript"/>
       <sz val="14"/>
-      <name val="Cordia New"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Cordia New"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="superscript"/>
-      <sz val="18"/>
       <name val="Cordia New"/>
       <family val="2"/>
     </font>
@@ -629,8 +617,41 @@
       <name val="Cordia New"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cordia New"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cordia New"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="CordiaUPC"/>
+      <family val="2"/>
+      <charset val="222"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Cordia New"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="18"/>
+      <name val="Cordia New"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +670,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="59">
     <border>
@@ -1346,7 +1379,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1384,13 +1417,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1401,17 +1428,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -1422,7 +1445,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -1453,46 +1475,41 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1505,10 +1522,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1517,19 +1534,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1547,10 +1564,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1559,8 +1576,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1570,28 +1604,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1599,10 +1615,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1619,10 +1635,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1651,16 +1673,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1669,10 +1691,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1687,16 +1709,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1726,13 +1748,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1747,16 +1769,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1771,28 +1793,28 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1836,6 +1858,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2500,8 +2543,8 @@
   </sheetPr>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="130" zoomScaleNormal="110" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="21"/>
@@ -2523,10 +2566,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102"/>
+      <c r="B1" s="103"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3" t="s">
         <v>1</v>
@@ -2566,429 +2609,429 @@
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="104"/>
+      <c r="F4" s="105"/>
       <c r="G4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="105" t="s">
+      <c r="H4" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="106"/>
+      <c r="I4" s="198"/>
     </row>
     <row r="5" spans="1:11" ht="28.5" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="107" t="s">
+      <c r="C5" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="109" t="s">
+      <c r="D5" s="107"/>
+      <c r="E5" s="201" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="195"/>
+      <c r="G5" s="196" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="110"/>
-      <c r="G5" s="21" t="s">
+      <c r="H5" s="199" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="200"/>
+      <c r="K5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H5" s="111" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="112"/>
-      <c r="K5" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="39.75" customHeight="1">
       <c r="A6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="122"/>
+      <c r="E6" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="107" t="s">
+      <c r="F6" s="124"/>
+      <c r="G6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="126" t="s">
+      <c r="H6" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="127"/>
-      <c r="G6" s="22" t="s">
+      <c r="I6" s="126"/>
+    </row>
+    <row r="7" spans="1:11" ht="28.5" customHeight="1" thickBot="1">
+      <c r="A7" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="128" t="s">
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="128"/>
+    </row>
+    <row r="8" spans="1:11" s="23" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="129"/>
-    </row>
-    <row r="7" spans="1:11" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A7" s="23" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="131"/>
-    </row>
-    <row r="8" spans="1:11" s="27" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="26" t="s">
+      <c r="I8" s="130"/>
+    </row>
+    <row r="9" spans="1:11" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="132" t="s">
+      <c r="B9" s="109"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="133"/>
-    </row>
-    <row r="9" spans="1:11" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="113" t="s">
+      <c r="F9" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="115"/>
-      <c r="E9" s="116" t="s">
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="115"/>
+    </row>
+    <row r="10" spans="1:11" ht="20.25" customHeight="1" thickTop="1">
+      <c r="A10" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="118" t="s">
+      <c r="B10" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="120"/>
-    </row>
-    <row r="10" spans="1:11" ht="20.25" customHeight="1" thickTop="1">
-      <c r="A10" s="29" t="s">
+      <c r="C10" s="117"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="121" t="s">
+      <c r="G10" s="27"/>
+      <c r="H10" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="122"/>
-      <c r="D10" s="123"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="30" t="s">
+      <c r="I10" s="120"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A11" s="137">
+        <v>1</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="124" t="s">
+      <c r="E11" s="90"/>
+      <c r="F11" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="125"/>
-    </row>
-    <row r="11" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A11" s="140">
-        <v>1</v>
-      </c>
-      <c r="B11" s="32" t="s">
+      <c r="G11" s="98"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A12" s="137"/>
+      <c r="B12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34" t="s">
+      <c r="E12" s="90"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A13" s="137"/>
+      <c r="B13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
-    </row>
-    <row r="12" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A12" s="140"/>
-      <c r="B12" s="32" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A13" s="140"/>
-      <c r="B13" s="19" t="s">
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A14" s="131">
+        <v>2</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42" t="s">
+      <c r="E14" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="45"/>
-    </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A14" s="134">
-        <v>2</v>
-      </c>
-      <c r="B14" s="32" t="s">
+      <c r="F14" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="142" t="s">
+      <c r="G14" s="29"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A15" s="138"/>
+      <c r="B15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="140"/>
+      <c r="F15" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="35"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="37"/>
-    </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A15" s="141"/>
-      <c r="B15" s="19" t="s">
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A16" s="137">
+        <v>3</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="143"/>
-      <c r="F15" s="46" t="s">
+      <c r="E16" s="90"/>
+      <c r="F16" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="45"/>
-    </row>
-    <row r="16" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A16" s="140">
-        <v>3</v>
-      </c>
-      <c r="B16" s="32" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A17" s="137"/>
+      <c r="B17" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="38" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="37"/>
-    </row>
-    <row r="17" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A17" s="140"/>
-      <c r="B17" s="19" t="s">
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38"/>
+    </row>
+    <row r="18" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A18" s="137">
+        <v>4</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="42" t="s">
+      <c r="E18" s="90"/>
+      <c r="F18" s="141">
+        <v>217</v>
+      </c>
+      <c r="G18" s="142"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A19" s="137"/>
+      <c r="B19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
-    </row>
-    <row r="18" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A18" s="140">
-        <v>4</v>
-      </c>
-      <c r="B18" s="32" t="s">
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="143"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="38"/>
+    </row>
+    <row r="20" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A20" s="137">
+        <v>5</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="144">
-        <v>217</v>
-      </c>
-      <c r="G18" s="145"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="37"/>
-    </row>
-    <row r="19" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A19" s="140"/>
-      <c r="B19" s="19" t="s">
+      <c r="E20" s="90"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A21" s="137"/>
+      <c r="B21" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="146"/>
-      <c r="G19" s="147"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="45"/>
-    </row>
-    <row r="20" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A20" s="140">
-        <v>5</v>
-      </c>
-      <c r="B20" s="32" t="s">
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="37"/>
-    </row>
-    <row r="21" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A21" s="140"/>
-      <c r="B21" s="19" t="s">
+      <c r="G21" s="43"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="38"/>
+    </row>
+    <row r="22" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A22" s="137">
+        <v>6</v>
+      </c>
+      <c r="B22" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="49" t="s">
+      <c r="E22" s="90"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A23" s="137"/>
+      <c r="B23" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="50"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-    </row>
-    <row r="22" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A22" s="140">
-        <v>6</v>
-      </c>
-      <c r="B22" s="32" t="s">
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="37"/>
-    </row>
-    <row r="23" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A23" s="140"/>
-      <c r="B23" s="19" t="s">
+      <c r="G23" s="45"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="38"/>
+    </row>
+    <row r="24" spans="1:13" s="48" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A24" s="131">
+        <v>7</v>
+      </c>
+      <c r="B24" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="51" t="s">
+      <c r="E24" s="92"/>
+      <c r="F24" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="45"/>
-    </row>
-    <row r="24" spans="1:13" s="55" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A24" s="134">
-        <v>7</v>
-      </c>
-      <c r="B24" s="54" t="s">
+      <c r="G24" s="146"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" spans="1:13" s="48" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A25" s="138"/>
+      <c r="B25" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="56"/>
-      <c r="F24" s="148" t="s">
+      <c r="E25" s="92"/>
+      <c r="F25" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="149"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="37"/>
-    </row>
-    <row r="25" spans="1:13" s="55" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A25" s="141"/>
-      <c r="B25" s="54" t="s">
+      <c r="G25" s="148"/>
+      <c r="H25" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="56"/>
-      <c r="F25" s="150" t="s">
+      <c r="I25" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="151"/>
-      <c r="H25" s="58" t="s">
+    </row>
+    <row r="26" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A26" s="131">
+        <v>8</v>
+      </c>
+      <c r="B26" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="I25" s="59" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="133" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A26" s="134">
-        <v>8</v>
-      </c>
-      <c r="B26" s="60" t="s">
+      <c r="G26" s="134"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="56"/>
+    </row>
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A27" s="132"/>
+      <c r="B27" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="136" t="s">
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="135" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="137"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="65"/>
-    </row>
-    <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A27" s="135"/>
-      <c r="B27" s="66" t="s">
+      <c r="G27" s="136"/>
+      <c r="H27" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1">
+      <c r="A28" s="61"/>
+      <c r="B28" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="138" t="s">
+      <c r="C28" s="117"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="27"/>
+      <c r="H28" s="119" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="120"/>
+    </row>
+    <row r="29" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A29" s="149">
+        <v>9</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="139"/>
-      <c r="H27" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="70" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1">
-      <c r="A28" s="71"/>
-      <c r="B28" s="121" t="s">
+      <c r="E29" s="139" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="150" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="122"/>
-      <c r="D28" s="123"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="31"/>
-      <c r="H28" s="124" t="s">
-        <v>29</v>
-      </c>
-      <c r="I28" s="125"/>
-    </row>
-    <row r="29" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A29" s="152">
-        <v>9</v>
-      </c>
-      <c r="B29" s="32" t="s">
+      <c r="G29" s="151"/>
+      <c r="H29" s="154" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="142" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="153" t="s">
+      <c r="I29" s="155"/>
+    </row>
+    <row r="30" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A30" s="138"/>
+      <c r="B30" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="154"/>
-      <c r="H29" s="157" t="s">
-        <v>65</v>
-      </c>
-      <c r="I29" s="158"/>
-    </row>
-    <row r="30" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A30" s="141"/>
-      <c r="B30" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="143"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="156"/>
-      <c r="H30" s="159"/>
-      <c r="I30" s="160"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="140"/>
+      <c r="F30" s="152"/>
+      <c r="G30" s="153"/>
+      <c r="H30" s="156"/>
+      <c r="I30" s="157"/>
       <c r="K30" s="1">
         <v>120</v>
       </c>
@@ -3000,21 +3043,21 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A31" s="140">
+      <c r="A31" s="137">
         <v>10</v>
       </c>
-      <c r="B31" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="33"/>
-      <c r="F31" s="164" t="s">
-        <v>68</v>
-      </c>
-      <c r="G31" s="165"/>
-      <c r="H31" s="168" t="s">
+      <c r="B31" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I31" s="169"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="161" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="162"/>
+      <c r="H31" s="165" t="s">
+        <v>63</v>
+      </c>
+      <c r="I31" s="166"/>
       <c r="K31" s="1">
         <v>3800</v>
       </c>
@@ -3026,34 +3069,34 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A32" s="140"/>
+      <c r="A32" s="137"/>
       <c r="B32" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="163"/>
+      <c r="G32" s="164"/>
+      <c r="H32" s="167"/>
+      <c r="I32" s="168"/>
+    </row>
+    <row r="33" spans="1:13" ht="18.75" customHeight="1">
+      <c r="A33" s="137">
+        <v>11</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="90"/>
+      <c r="F33" s="169" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="166"/>
-      <c r="G32" s="167"/>
-      <c r="H32" s="170"/>
-      <c r="I32" s="171"/>
-    </row>
-    <row r="33" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A33" s="140">
-        <v>11</v>
-      </c>
-      <c r="B33" s="32" t="s">
+      <c r="G33" s="170"/>
+      <c r="H33" s="165" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="172" t="s">
-        <v>71</v>
-      </c>
-      <c r="G33" s="173"/>
-      <c r="H33" s="168" t="s">
-        <v>72</v>
-      </c>
-      <c r="I33" s="169"/>
+      <c r="I33" s="166"/>
       <c r="K33" s="1">
         <f>K31/K30</f>
         <v>31.666666666666668</v>
@@ -3068,215 +3111,215 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A34" s="140"/>
+      <c r="A34" s="137"/>
       <c r="B34" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="171"/>
+      <c r="G34" s="172"/>
+      <c r="H34" s="167"/>
+      <c r="I34" s="168"/>
+    </row>
+    <row r="35" spans="1:13" s="48" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A35" s="131">
+        <v>12</v>
+      </c>
+      <c r="B35" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="173" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="174"/>
-      <c r="G34" s="175"/>
-      <c r="H34" s="170"/>
-      <c r="I34" s="171"/>
-    </row>
-    <row r="35" spans="1:13" s="55" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A35" s="134">
-        <v>12</v>
-      </c>
-      <c r="B35" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="176" t="s">
-        <v>75</v>
-      </c>
-      <c r="G35" s="177"/>
-      <c r="H35" s="178"/>
-      <c r="I35" s="179"/>
-      <c r="L35" s="55">
+      <c r="G35" s="174"/>
+      <c r="H35" s="175"/>
+      <c r="I35" s="176"/>
+      <c r="L35" s="48">
         <f>K33-M33</f>
         <v>3.7407407407407405</v>
       </c>
-      <c r="M35" s="55">
+      <c r="M35" s="48">
         <f>L33-K33</f>
         <v>4.8095238095238066</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="55" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="152"/>
-      <c r="B36" s="54" t="s">
+    <row r="36" spans="1:13" s="48" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A36" s="149"/>
+      <c r="B36" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="92"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="178"/>
+      <c r="H36" s="179"/>
+      <c r="I36" s="180"/>
+    </row>
+    <row r="37" spans="1:13" s="48" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A37" s="63"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="159"/>
+      <c r="H37" s="158"/>
+      <c r="I37" s="160"/>
+    </row>
+    <row r="38" spans="1:13" ht="21" customHeight="1">
+      <c r="A38" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="22"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="67"/>
+    </row>
+    <row r="39" spans="1:13" ht="2.25" customHeight="1">
+      <c r="A39" s="69"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="67"/>
+    </row>
+    <row r="40" spans="1:13" ht="0.75" customHeight="1">
+      <c r="A40" s="69"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="67"/>
+    </row>
+    <row r="41" spans="1:13" ht="19.5" customHeight="1">
+      <c r="A41" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="E36" s="56"/>
-      <c r="F36" s="180"/>
-      <c r="G36" s="181"/>
-      <c r="H36" s="182"/>
-      <c r="I36" s="183"/>
-    </row>
-    <row r="37" spans="1:13" s="55" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A37" s="74"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="161"/>
-      <c r="G37" s="162"/>
-      <c r="H37" s="161"/>
-      <c r="I37" s="163"/>
-    </row>
-    <row r="38" spans="1:13" ht="21" customHeight="1">
-      <c r="A38" s="78" t="s">
+      <c r="B41" s="71"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="79"/>
-    </row>
-    <row r="39" spans="1:13" ht="2.25" customHeight="1">
-      <c r="A39" s="81"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="79"/>
-    </row>
-    <row r="40" spans="1:13" ht="0.75" customHeight="1">
-      <c r="A40" s="81"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="80"/>
-      <c r="H40" s="79"/>
-    </row>
-    <row r="41" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A41" s="82" t="s">
+      <c r="G41" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="83"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="84" t="s">
+      <c r="H41" s="181" t="s">
         <v>79</v>
       </c>
-      <c r="G41" s="85" t="s">
+      <c r="I41" s="182"/>
+    </row>
+    <row r="42" spans="1:13" s="78" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A42" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="H41" s="184" t="s">
+      <c r="B42" s="75"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="183" t="s">
         <v>81</v>
       </c>
-      <c r="I41" s="185"/>
-    </row>
-    <row r="42" spans="1:13" s="90" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A42" s="86" t="s">
+      <c r="G42" s="76"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="77"/>
+    </row>
+    <row r="43" spans="1:13" ht="20.25" customHeight="1">
+      <c r="A43" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="87"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="186" t="s">
+      <c r="B43" s="75"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="184"/>
+      <c r="G43" s="79"/>
+      <c r="H43" s="186"/>
+      <c r="I43" s="187"/>
+    </row>
+    <row r="44" spans="1:13" ht="24.75" customHeight="1">
+      <c r="A44" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="G42" s="88"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="89"/>
-    </row>
-    <row r="43" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A43" s="86" t="s">
+      <c r="B44" s="75"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="185"/>
+      <c r="G44" s="80" t="s">
+        <v>81</v>
+      </c>
+      <c r="H44" s="188" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="87"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="187"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="189"/>
-      <c r="I43" s="190"/>
-    </row>
-    <row r="44" spans="1:13" ht="24.75" customHeight="1">
-      <c r="A44" s="86" t="s">
+      <c r="I44" s="189"/>
+    </row>
+    <row r="45" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A45" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="87"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="188"/>
-      <c r="G44" s="92" t="s">
-        <v>83</v>
-      </c>
-      <c r="H44" s="191" t="s">
+      <c r="B45" s="75"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="190" t="s">
         <v>86</v>
       </c>
-      <c r="I44" s="192"/>
-    </row>
-    <row r="45" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A45" s="86" t="s">
+      <c r="G45" s="81"/>
+      <c r="H45" s="82"/>
+      <c r="I45" s="14"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="87"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="193" t="s">
+      <c r="B46" s="75"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="191"/>
+      <c r="G46" s="81"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="38"/>
+    </row>
+    <row r="47" spans="1:13" ht="21.6" thickBot="1">
+      <c r="A47" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="G45" s="93"/>
-      <c r="H45" s="94"/>
-      <c r="I45" s="14"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="86" t="s">
+      <c r="B47" s="85"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="192"/>
+      <c r="G47" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="87"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="194"/>
-      <c r="G46" s="93"/>
-      <c r="H46" s="95"/>
-      <c r="I46" s="45"/>
-    </row>
-    <row r="47" spans="1:13" ht="21.6" thickBot="1">
-      <c r="A47" s="96" t="s">
+      <c r="H47" s="193" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="97"/>
-      <c r="C47" s="98"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="98"/>
-      <c r="F47" s="195"/>
-      <c r="G47" s="99" t="s">
+      <c r="I47" s="194"/>
+    </row>
+    <row r="48" spans="1:13" ht="22.2" thickTop="1" thickBot="1">
+      <c r="A48" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="H47" s="196" t="s">
+      <c r="B48" s="89"/>
+      <c r="H48" s="113" t="s">
         <v>92</v>
       </c>
-      <c r="I47" s="197"/>
-    </row>
-    <row r="48" spans="1:13" ht="22.2" thickTop="1" thickBot="1">
-      <c r="A48" s="100" t="s">
-        <v>93</v>
-      </c>
-      <c r="B48" s="101"/>
-      <c r="H48" s="118" t="s">
-        <v>94</v>
-      </c>
-      <c r="I48" s="120"/>
+      <c r="I48" s="115"/>
     </row>
     <row r="49" ht="21.6" thickTop="1"/>
   </sheetData>

</xml_diff>